<commit_message>
Run w new acid pH, add acid red plot
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -139,11 +139,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -166,19 +167,20 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3465A4"/>
+      <name val="Sans"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,7 +230,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,6 +247,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -252,7 +318,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,7 +359,7 @@
       <c r="D2" s="1" t="n">
         <v>3.9</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="3" t="n">
         <v>7.2</v>
       </c>
     </row>
@@ -310,7 +376,7 @@
       <c r="D3" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="3" t="n">
         <v>7</v>
       </c>
     </row>
@@ -327,7 +393,7 @@
       <c r="D4" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="3" t="n">
         <v>7.9</v>
       </c>
     </row>
@@ -344,8 +410,9 @@
       <c r="D5" s="1" t="n">
         <v>3.9</v>
       </c>
-      <c r="E5" s="3" t="n">
-        <v>6.6</v>
+      <c r="E5" s="4" t="n">
+        <f aca="false">E2-0.73</f>
+        <v>6.47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -361,8 +428,9 @@
       <c r="D6" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="E6" s="3" t="n">
-        <v>6.4</v>
+      <c r="E6" s="4" t="n">
+        <f aca="false">E3-0.53</f>
+        <v>6.47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,8 +446,9 @@
       <c r="D7" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E7" s="3" t="n">
-        <v>6.6</v>
+      <c r="E7" s="4" t="n">
+        <f aca="false">E4-1.38</f>
+        <v>6.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add comparison to report EFs
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -42,7 +42,7 @@
     <t xml:space="preserve">Svinegylle</t>
   </si>
   <si>
-    <t xml:space="preserve">pig</t>
+    <t xml:space="preserve">Pig</t>
   </si>
   <si>
     <t xml:space="preserve">FALSE</t>
@@ -51,13 +51,13 @@
     <t xml:space="preserve">Kvæggylle</t>
   </si>
   <si>
-    <t xml:space="preserve">cattle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Agfasset biomasse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mix</t>
+    <t xml:space="preserve">Cattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afgasset biomasse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digestate</t>
   </si>
   <si>
     <t xml:space="preserve">TRUE</t>
@@ -117,22 +117,22 @@
     <t xml:space="preserve">app.rate.ni</t>
   </si>
   <si>
-    <t xml:space="preserve">bsth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shallow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">os</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cs</t>
+    <t xml:space="preserve">Trailing hose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open slot injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed slot injection</t>
   </si>
 </sst>
 </file>
@@ -317,8 +317,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -603,13 +603,14 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="2" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,7 +638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -651,7 +652,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Use different months for summer for bsth, os, cs
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t xml:space="preserve">man.name</t>
   </si>
@@ -69,6 +69,9 @@
     <t xml:space="preserve">app.timing</t>
   </si>
   <si>
+    <t xml:space="preserve">app.mthd.wthr</t>
+  </si>
+  <si>
     <t xml:space="preserve">air.temp</t>
   </si>
   <si>
@@ -78,12 +81,18 @@
     <t xml:space="preserve">rain.rate</t>
   </si>
   <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marts</t>
   </si>
   <si>
     <t xml:space="preserve">March</t>
   </si>
   <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
     <t xml:space="preserve">April</t>
   </si>
   <si>
@@ -99,12 +108,33 @@
     <t xml:space="preserve">Summer</t>
   </si>
   <si>
+    <t xml:space="preserve">Trailing hose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For trailing hose, 6-8.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Efterår</t>
   </si>
   <si>
     <t xml:space="preserve">Autumn</t>
   </si>
   <si>
+    <t xml:space="preserve">9 (September)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open slot injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summer-grass, for open slot injection, 5-8.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closed slot injection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summer, before winter rapeseed, for closed slot injection, 7-8.</t>
+  </si>
+  <si>
     <t xml:space="preserve">app.mthd</t>
   </si>
   <si>
@@ -117,9 +147,6 @@
     <t xml:space="preserve">app.rate.ni</t>
   </si>
   <si>
-    <t xml:space="preserve">Trailing hose</t>
-  </si>
-  <si>
     <t xml:space="preserve">None</t>
   </si>
   <si>
@@ -127,12 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">Deep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open slot injection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Closed slot injection</t>
   </si>
 </sst>
 </file>
@@ -467,20 +488,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,90 +522,163 @@
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="n">
         <v>4.9</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="E2" s="1" t="n">
         <v>4.025</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="n">
         <v>8.5</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="E3" s="1" t="n">
         <v>3.91</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="D4" s="1" t="n">
         <v>12.4</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="E4" s="1" t="n">
         <v>3.565</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>16.867</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="E5" s="1" t="n">
         <v>3.18167</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.09</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>14.6</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="E6" s="1" t="n">
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>15.75</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>3.2775</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>0.09</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>17.55</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>3.105</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -603,8 +699,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,24 +711,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>30</v>
@@ -640,10 +736,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>4</v>
@@ -654,10 +750,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>4</v>
@@ -668,10 +764,10 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -679,10 +775,10 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Revert "Use different months for summer for bsth, os, cs"
This reverts commit a7df5d03242e2267afa1364533f4fb0604e6ff94.

Correct misunderstanding with AP. We decided to actually use same months for all application methods for summer.
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t xml:space="preserve">man.name</t>
   </si>
@@ -69,9 +69,6 @@
     <t xml:space="preserve">app.timing</t>
   </si>
   <si>
-    <t xml:space="preserve">app.mthd.wthr</t>
-  </si>
-  <si>
     <t xml:space="preserve">air.temp</t>
   </si>
   <si>
@@ -81,18 +78,12 @@
     <t xml:space="preserve">rain.rate</t>
   </si>
   <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marts</t>
   </si>
   <si>
     <t xml:space="preserve">March</t>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
     <t xml:space="preserve">April</t>
   </si>
   <si>
@@ -108,52 +99,40 @@
     <t xml:space="preserve">Summer</t>
   </si>
   <si>
+    <t xml:space="preserve">Efterår</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autumn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.mthd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t.incorp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app.rate.ni</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trailing hose</t>
   </si>
   <si>
-    <t xml:space="preserve">For trailing hose, 6-8.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efterår</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autumn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9 (September)</t>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep</t>
   </si>
   <si>
     <t xml:space="preserve">Open slot injection</t>
   </si>
   <si>
-    <t xml:space="preserve">Summer-grass, for open slot injection, 5-8.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Closed slot injection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Summer, before winter rapeseed, for closed slot injection, 7-8.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.mthd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incorp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t.incorp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">app.rate.ni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shallow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deep</t>
   </si>
 </sst>
 </file>
@@ -488,22 +467,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,163 +499,90 @@
       <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>4.9</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>4.9</v>
+        <v>4.025</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>4.025</v>
-      </c>
-      <c r="F2" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>8.5</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>8.5</v>
+        <v>3.91</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>3.91</v>
-      </c>
-      <c r="F3" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="C4" s="1" t="n">
+        <v>12.4</v>
+      </c>
       <c r="D4" s="1" t="n">
-        <v>12.4</v>
+        <v>3.565</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>3.565</v>
-      </c>
-      <c r="F4" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>16.867</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>16.867</v>
+        <v>3.18167</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>3.18167</v>
-      </c>
-      <c r="F5" s="1" t="n">
         <v>0.09</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>14.6</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>14.6</v>
+        <v>3.45</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="F6" s="1" t="n">
         <v>0.09</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>15.75</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>3.2775</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>17.55</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>3.105</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -699,8 +603,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -711,24 +615,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>30</v>
@@ -736,10 +640,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>4</v>
@@ -750,10 +654,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>4</v>
@@ -764,10 +668,10 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -775,10 +679,10 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Simplify inputs and code, rely on prepDat()
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -22,10 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
-  <si>
-    <t xml:space="preserve">man.name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t xml:space="preserve">man.source</t>
   </si>
@@ -42,30 +39,18 @@
     <t xml:space="preserve">Svinegylle</t>
   </si>
   <si>
-    <t xml:space="preserve">Pig</t>
-  </si>
-  <si>
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">Kvæggylle</t>
   </si>
   <si>
-    <t xml:space="preserve">Cattle</t>
-  </si>
-  <si>
     <t xml:space="preserve">Afgasset biomasse</t>
   </si>
   <si>
-    <t xml:space="preserve">Digestate</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRUE</t>
   </si>
   <si>
-    <t xml:space="preserve">app.timing.dk</t>
-  </si>
-  <si>
     <t xml:space="preserve">app.timing</t>
   </si>
   <si>
@@ -81,28 +66,16 @@
     <t xml:space="preserve">Marts</t>
   </si>
   <si>
-    <t xml:space="preserve">March</t>
-  </si>
-  <si>
     <t xml:space="preserve">April</t>
   </si>
   <si>
     <t xml:space="preserve">Maj</t>
   </si>
   <si>
-    <t xml:space="preserve">May</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sommer</t>
   </si>
   <si>
-    <t xml:space="preserve">Summer</t>
-  </si>
-  <si>
     <t xml:space="preserve">Efterår</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autumn</t>
   </si>
   <si>
     <t xml:space="preserve">app.mthd</t>
@@ -315,139 +288,117 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.22"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="1" t="n">
         <v>3.9</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="D2" s="3" t="n">
         <v>7.2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="D3" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="D4" s="3" t="n">
         <v>7.9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>3.9</v>
       </c>
-      <c r="E5" s="4" t="n">
-        <f aca="false">E2-0.73</f>
+      <c r="D5" s="4" t="n">
+        <f aca="false">D2-0.73</f>
         <v>6.47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="n">
+      <c r="C6" s="1" t="n">
         <v>6.5</v>
       </c>
-      <c r="E6" s="4" t="n">
-        <f aca="false">E3-0.53</f>
+      <c r="D6" s="4" t="n">
+        <f aca="false">D3-0.53</f>
         <v>6.47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="n">
         <v>5.1</v>
       </c>
-      <c r="E7" s="4" t="n">
-        <f aca="false">E4-1.38</f>
+      <c r="D7" s="4" t="n">
+        <f aca="false">D4-1.38</f>
         <v>6.52</v>
       </c>
     </row>
@@ -467,121 +418,102 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="5" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>4.9</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>4.9</v>
+        <v>4.025</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>4.025</v>
-      </c>
-      <c r="E2" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>8.5</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>8.5</v>
+        <v>3.91</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>3.91</v>
-      </c>
-      <c r="E3" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>12.4</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>12.4</v>
+        <v>3.565</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>3.565</v>
-      </c>
-      <c r="E4" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>16.867</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>16.867</v>
+        <v>3.18167</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>3.18167</v>
-      </c>
-      <c r="E5" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>14.6</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>14.6</v>
+        <v>3.45</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="E6" s="1" t="n">
         <v>0.09</v>
       </c>
     </row>
@@ -615,24 +547,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>30</v>
@@ -640,10 +572,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>4</v>
@@ -654,10 +586,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>4</v>
@@ -668,10 +600,10 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>0</v>
@@ -679,10 +611,10 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Vary rain by month
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -109,10 +109,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -187,7 +188,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,6 +206,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -417,8 +422,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -455,7 +460,7 @@
         <v>4.025</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.09</v>
+        <v>0.074</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,8 +473,8 @@
       <c r="C3" s="1" t="n">
         <v>3.91</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>0.09</v>
+      <c r="D3" s="5" t="n">
+        <v>0.06</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,7 +488,7 @@
         <v>3.565</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.09</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,8 +501,8 @@
       <c r="C5" s="1" t="n">
         <v>3.18167</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>0.09</v>
+      <c r="D5" s="3" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -511,7 +516,7 @@
         <v>3.45</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>0.09</v>
+        <v>0.13</v>
       </c>
     </row>
   </sheetData>
@@ -532,7 +537,7 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New monthly rainfall rates
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -423,7 +423,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,7 +460,7 @@
         <v>4.025</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.074</v>
+        <v>0.056</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,7 +474,7 @@
         <v>3.91</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +488,7 @@
         <v>3.565</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>0.066</v>
+        <v>0.072</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,7 +502,7 @@
         <v>3.18167</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Use newest weather inputs.
Include monthly means for rain
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -113,7 +113,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,70 +453,70 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>4.025</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.056</v>
+      <c r="B2" s="5" t="n">
+        <v>4.2751882725795</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>4.04186842718138</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.0556576719496239</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>3.91</v>
+      <c r="B3" s="5" t="n">
+        <v>8.19748979894988</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>3.81357212945869</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.12</v>
+        <v>0.116938350042087</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>12.4</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>3.565</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.072</v>
+      <c r="B4" s="5" t="n">
+        <v>12.3751389561464</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>3.45567498501387</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.071780395514249</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>16.867</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>3.18167</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0.11</v>
+      <c r="B5" s="5" t="n">
+        <v>16.8185301623819</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>3.10883875876392</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.107050334741296</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>14.6</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>3.45</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.13</v>
+      <c r="B6" s="5" t="n">
+        <v>14.3971459030677</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>3.30879945612945</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.128927644374806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use simpler weather means
</commit_message>
<xml_diff>
--- a/2021-0294105_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_EFs/inputs/inputs.xlsx
@@ -423,7 +423,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -454,13 +454,13 @@
         <v>13</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>4.43852385594436</v>
+        <v>4.43101207056639</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>4.05876346426737</v>
+        <v>4.05891613991413</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.0591167836218906</v>
+        <v>0.0599629009095261</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -468,13 +468,13 @@
         <v>14</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>8.25492234102729</v>
+        <v>8.23645983645984</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>3.84140710160771</v>
+        <v>3.84445591865745</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.103059242668137</v>
+        <v>0.0552119412831931</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,13 +482,13 @@
         <v>15</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>12.4451874039939</v>
+        <v>12.4492495309568</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>3.47437423735091</v>
+        <v>3.48391526295633</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.0708223837251174</v>
+        <v>0.0702993488962998</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,13 +496,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>16.8746331383993</v>
+        <v>16.8762259816193</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>3.15328236349691</v>
+        <v>3.15624012423227</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.10575888684737</v>
+        <v>0.105925308296069</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,13 +510,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>14.4940673234811</v>
+        <v>14.4977479635841</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>3.3202994261131</v>
+        <v>3.32276959833633</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0.128483843537415</v>
+        <v>0.128260170445409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>